<commit_message>
Till 2nd Feb 2021
</commit_message>
<xml_diff>
--- a/data/process_13/inputData.xlsx
+++ b/data/process_13/inputData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tspiinfotech-my.sharepoint.com/personal/asrivastava_tsp_tech/Documents/Documents/UiPath/BDG/data/process_13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asrivastava\OneDrive - TSPI Infotech Pvt Ltd\Documents\UiPath\BDG\data\process_13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Process 3" sheetId="8" r:id="rId8"/>
     <sheet name="Process 2" sheetId="5" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2262,7 +2262,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2417,7 +2417,7 @@
         <v>71</v>
       </c>
       <c r="E8" s="12">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="F8" s="50"/>
       <c r="G8" s="1"/>
@@ -6232,6 +6232,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FFE358E4433FD84A9A34523DAB00F7EB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8f3f11fdb443e8b4b1a57d51f2ae48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="627e885a-4408-46af-8180-28ca0c06a43e" xmlns:ns3="bbd7ad43-7622-4e03-bc1d-5f6f87a52367" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9878c85569a301255d672f426fac71ea" ns2:_="" ns3:_="">
     <xsd:import namespace="627e885a-4408-46af-8180-28ca0c06a43e"/>
@@ -6442,22 +6457,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84DCB23-466D-4EDB-95EF-6AF2F90EC447}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="627e885a-4408-46af-8180-28ca0c06a43e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bbd7ad43-7622-4e03-bc1d-5f6f87a52367"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E5D96F2-FF42-407F-9756-AD782ED49C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E02152-A7A6-4163-B9A8-7E722AB35DEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6474,29 +6499,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E5D96F2-FF42-407F-9756-AD782ED49C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84DCB23-466D-4EDB-95EF-6AF2F90EC447}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bbd7ad43-7622-4e03-bc1d-5f6f87a52367"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="627e885a-4408-46af-8180-28ca0c06a43e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>